<commit_message>
Login e cadastro validados
</commit_message>
<xml_diff>
--- a/Documentação/Documentação/TI-Backlog-Grupo10.xlsx
+++ b/Documentação/Documentação/TI-Backlog-Grupo10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivia\Projeto\projeto-pi\Documentação\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7837E0A1-EC4C-43C0-AAB9-F92E9E4E8307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0AFE22-D1D6-4D3D-B994-8C2B4A2D8B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{0E4C50FC-4743-41E1-8EF2-E2C48055392E}"/>
   </bookViews>
@@ -1745,9 +1745,9 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:f>BackLog!$L$3:$L$7</c:f>
-            </c:strRef>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1833,9 +1833,9 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:f>BackLog!$L$3:$L$7</c:f>
-            </c:strRef>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2967,8 +2967,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3613,7 +3613,7 @@
         <v>29</v>
       </c>
       <c r="H18" s="44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Arrumei o CSS da calculadora
</commit_message>
<xml_diff>
--- a/Documentação/Documentação/TI-Backlog-Grupo10.xlsx
+++ b/Documentação/Documentação/TI-Backlog-Grupo10.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivia\Projeto\projeto-pi\Documentação\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivia\projeto\projeto-pi\Documentação\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66ED818D-3F46-4FC1-9BC7-EB93CFC53CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACD889B-2784-4ADA-A47D-64D58B9A0B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{0E4C50FC-4743-41E1-8EF2-E2C48055392E}"/>
   </bookViews>
@@ -1030,140 +1030,7 @@
     <cellStyle name="Feito" xfId="1" xr:uid="{5B153B00-796B-4D41-98D1-35BE0DB48071}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="44">
     <dxf>
       <font>
         <b/>
@@ -3173,7 +3040,7 @@
   <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4112,7 +3979,7 @@
         <v>29</v>
       </c>
       <c r="H26" s="44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I26" s="14" t="s">
         <v>34</v>
@@ -4717,41 +4584,41 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="C3:C44">
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Desejável">
+    <cfRule type="containsText" dxfId="43" priority="2" operator="containsText" text="Desejável">
       <formula>NOT(ISERROR(SEARCH("Desejável",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="Importante">
+    <cfRule type="containsText" dxfId="42" priority="3" operator="containsText" text="Importante">
       <formula>NOT(ISERROR(SEARCH("Importante",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="Essencial">
+    <cfRule type="containsText" dxfId="41" priority="4" operator="containsText" text="Essencial">
       <formula>NOT(ISERROR(SEARCH("Essencial",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D44">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="PP">
+    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="PP">
       <formula>NOT(ISERROR(SEARCH("PP",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="GG">
+    <cfRule type="containsText" dxfId="39" priority="5" operator="containsText" text="GG">
       <formula>NOT(ISERROR(SEARCH("GG",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="G">
+    <cfRule type="containsText" dxfId="38" priority="6" operator="containsText" text="G">
       <formula>NOT(ISERROR(SEARCH("G",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="M">
+    <cfRule type="containsText" dxfId="37" priority="7" operator="containsText" text="M">
       <formula>NOT(ISERROR(SEARCH("M",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="36" priority="8" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H44">
-    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Pendente">
+    <cfRule type="containsText" dxfId="35" priority="9" operator="containsText" text="Pendente">
       <formula>NOT(ISERROR(SEARCH("Pendente",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="Em andamento">
+    <cfRule type="containsText" dxfId="34" priority="10" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Feito">
+    <cfRule type="containsText" dxfId="33" priority="11" operator="containsText" text="Feito">
       <formula>NOT(ISERROR(SEARCH("Feito",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5183,41 +5050,41 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="C3:C12">
-    <cfRule type="containsText" dxfId="54" priority="2" operator="containsText" text="Desejável">
+    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="Desejável">
       <formula>NOT(ISERROR(SEARCH("Desejável",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="3" operator="containsText" text="Importante">
+    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="Importante">
       <formula>NOT(ISERROR(SEARCH("Importante",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="4" operator="containsText" text="Essencial">
+    <cfRule type="containsText" dxfId="30" priority="4" operator="containsText" text="Essencial">
       <formula>NOT(ISERROR(SEARCH("Essencial",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D12">
-    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="PP">
+    <cfRule type="containsText" dxfId="29" priority="1" operator="containsText" text="PP">
       <formula>NOT(ISERROR(SEARCH("PP",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="5" operator="containsText" text="GG">
+    <cfRule type="containsText" dxfId="28" priority="5" operator="containsText" text="GG">
       <formula>NOT(ISERROR(SEARCH("GG",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="6" operator="containsText" text="G">
+    <cfRule type="containsText" dxfId="27" priority="6" operator="containsText" text="G">
       <formula>NOT(ISERROR(SEARCH("G",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="7" operator="containsText" text="M">
+    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="M">
       <formula>NOT(ISERROR(SEARCH("M",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="8" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="25" priority="8" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H12">
-    <cfRule type="containsText" dxfId="46" priority="9" operator="containsText" text="Pendente">
+    <cfRule type="containsText" dxfId="24" priority="9" operator="containsText" text="Pendente">
       <formula>NOT(ISERROR(SEARCH("Pendente",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="10" operator="containsText" text="Em andamento">
+    <cfRule type="containsText" dxfId="23" priority="10" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="11" operator="containsText" text="Feito">
+    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="Feito">
       <formula>NOT(ISERROR(SEARCH("Feito",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5807,41 +5674,41 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C17">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Desejável">
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Desejável">
       <formula>NOT(ISERROR(SEARCH("Desejável",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Importante">
+    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="Importante">
       <formula>NOT(ISERROR(SEARCH("Importante",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Essencial">
+    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="Essencial">
       <formula>NOT(ISERROR(SEARCH("Essencial",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D17">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="PP">
+    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="PP">
       <formula>NOT(ISERROR(SEARCH("PP",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="GG">
+    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="GG">
       <formula>NOT(ISERROR(SEARCH("GG",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="G">
+    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="G">
       <formula>NOT(ISERROR(SEARCH("G",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="M">
+    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="M">
       <formula>NOT(ISERROR(SEARCH("M",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H17">
-    <cfRule type="containsText" dxfId="2" priority="9" operator="containsText" text="Pendente">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Pendente">
       <formula>NOT(ISERROR(SEARCH("Pendente",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="10" operator="containsText" text="Em andamento">
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="11" operator="containsText" text="Feito">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Feito">
       <formula>NOT(ISERROR(SEARCH("Feito",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6474,41 +6341,41 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C19">
-    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="Desejável">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Desejável">
       <formula>NOT(ISERROR(SEARCH("Desejável",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="Importante">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Importante">
       <formula>NOT(ISERROR(SEARCH("Importante",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="4" operator="containsText" text="Essencial">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Essencial">
       <formula>NOT(ISERROR(SEARCH("Essencial",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D19">
-    <cfRule type="containsText" dxfId="29" priority="1" operator="containsText" text="PP">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="PP">
       <formula>NOT(ISERROR(SEARCH("PP",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="5" operator="containsText" text="GG">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="GG">
       <formula>NOT(ISERROR(SEARCH("GG",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="6" operator="containsText" text="G">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="G">
       <formula>NOT(ISERROR(SEARCH("G",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="M">
+    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="M">
       <formula>NOT(ISERROR(SEARCH("M",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="8" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H19">
-    <cfRule type="containsText" dxfId="24" priority="9" operator="containsText" text="Pendente">
+    <cfRule type="containsText" dxfId="2" priority="9" operator="containsText" text="Pendente">
       <formula>NOT(ISERROR(SEARCH("Pendente",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="10" operator="containsText" text="Em andamento">
+    <cfRule type="containsText" dxfId="1" priority="10" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="Feito">
+    <cfRule type="containsText" dxfId="0" priority="11" operator="containsText" text="Feito">
       <formula>NOT(ISERROR(SEARCH("Feito",H3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>